<commit_message>
add and adjust: Add ->  data_load_dados_recebidos and adjust tratamento_gold and silver and add carga dados on pipeline_dados_recebidos
</commit_message>
<xml_diff>
--- a/Case 1 - Dados Fin/Dados Financeiros - Estrutura HData.xlsx
+++ b/Case 1 - Dados Fin/Dados Financeiros - Estrutura HData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://falconi365.sharepoint.com/sites/H-DataGovernanaClnicaDigitalTeam-CoordenaesHData/Documentos Compartilhados/Coordenações HData/Recrutamento e Seleção/Engenharia de Dados/Case Aplicado 202309/Case Aplicado/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/33e41e1f1e2420ca/Documentos/Projetos/HData/Case 1 - Dados Fin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{C3BE2095-7AFB-42A9-B9E0-07D4EF17CF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A23D722-CBEF-4AA2-A6D6-3E606600AADC}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{C3BE2095-7AFB-42A9-B9E0-07D4EF17CF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBD92650-939B-4003-9191-4329B8B5BF77}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="880" activeTab="1" xr2:uid="{FD72B0E9-57D9-4606-B900-E86AD6F62B7A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="880" activeTab="1" xr2:uid="{FD72B0E9-57D9-4606-B900-E86AD6F62B7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fluxo Caixa - Planilha Padrao" sheetId="9" r:id="rId1"/>
@@ -552,13 +552,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3911</xdr:colOff>
+      <xdr:colOff>80111</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>592696</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>59296</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>16283</xdr:rowOff>
     </xdr:to>
@@ -583,8 +583,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4591151" y="0"/>
-          <a:ext cx="10342385" cy="5769383"/>
+          <a:off x="4667351" y="0"/>
+          <a:ext cx="10342385" cy="5761763"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -597,9 +597,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -637,7 +637,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -743,7 +743,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -885,7 +885,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1968,18 +1968,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2121,6 +2121,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07D9415-3DFF-4BD7-BEE7-C7EA3D1708D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37EF911B-9C9D-4FB7-BABC-DE221DE7D378}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2129,14 +2137,6 @@
     <ds:schemaRef ds:uri="e17094b4-5e31-4993-b967-7c52cd53587b"/>
     <ds:schemaRef ds:uri="227f0239-8b52-43ba-ac76-d573c5d0ac85"/>
     <ds:schemaRef ds:uri="a46526b5-c3bd-47a4-b164-544ce4984736"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07D9415-3DFF-4BD7-BEE7-C7EA3D1708D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>